<commit_message>
Update return shipments data (auto)
</commit_message>
<xml_diff>
--- a/docs/data/returns_intransit.xlsx
+++ b/docs/data/returns_intransit.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,150 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>No new InTransit trackings (deduped for 30 days).</t>
+          <t>tracking_number</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>carrier_slug</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>status_tag</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>title</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>order_id</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>last_checkpoint_time</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>last_checkpoint_location</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>updated_at</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TEST_GDPR</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>dbschenker-se</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>SHIPMENT_TITLE</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2026-02-08T12:16:34+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TEST_TRACKING_DECEMBER</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dhl</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>TEST_Tracking_December</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2026-02-08T11:24:55+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TEST_TRACKING</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>kn</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ZFRE</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>2026-02-08T11:24:18+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ITD-0-12345678</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>testing-courier</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Delivered</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>ITD-0-12345678</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>2026-02-08T11:07:24+00:00</t>
         </is>
       </c>
     </row>

</xml_diff>